<commit_message>
added the the Gini coefficient and gain chart
</commit_message>
<xml_diff>
--- a/KS statistic.xlsx
+++ b/KS statistic.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\customer\Desktop\Taipa\PhD\PD\Scorecard\IFRS9Udemy\LifetimePD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\customer\Desktop\Taipa\PhD\PD\Scorecard\CreditScore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B855881-7840-4FC5-9A85-46C53E4922EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457752EE-BE11-4B4C-B226-9CC2BE7EBF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{19B16C6B-3CF0-41B8-9609-6745485D9333}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>bs</t>
   </si>
@@ -84,6 +85,21 @@
   </si>
   <si>
     <t>Gini Coeficient = 100% - Sum(Z)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorenz curve </t>
+  </si>
+  <si>
+    <t>Gini</t>
+  </si>
+  <si>
+    <t>c-statistic</t>
+  </si>
+  <si>
+    <t>.= (1+ Gini)/2</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -301,6 +317,1961 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Lorenz</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Curve</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumm % Total Good </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25974025974025972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54545454545454541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70129870129870131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8701298701298702</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89610389610389618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92207792207792216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97402597402597413</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97402597402597413</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.628</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.876</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B88E-471D-BA7C-3E7F5F24F1C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1750341983"/>
+        <c:axId val="1750352543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1750341983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750352543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1750352543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750341983"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Gains Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cumm % Total Bad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$22:$L$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$22:$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25974025974025972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54545454545454541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70129870129870131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81818181818181823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8701298701298702</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89610389610389618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92207792207792216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97402597402597413</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97402597402597413</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C37-4BC1-A30B-798C49854045}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1750325663"/>
+        <c:axId val="1750301663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1750325663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750301663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1750301663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750325663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB654748-5AFE-3E24-1C09-50B81988ABB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A97CF9C-65AF-AB22-3EFF-1344F368D2F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -618,10 +2589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682D2D10-AC95-41EB-8BBD-0E1D690E692B}">
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +2777,7 @@
         <v>0.70129870129870131</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J11" si="6">J4+H5</f>
+        <f t="shared" ref="J5:J10" si="6">J4+H5</f>
         <v>0.17599999999999999</v>
       </c>
       <c r="K5" s="11">
@@ -814,11 +2785,11 @@
         <v>0.52529870129870138</v>
       </c>
       <c r="L5" s="11">
-        <f t="shared" ref="L5:L12" si="7">I5-I4</f>
+        <f t="shared" ref="L5:L11" si="7">I5-I4</f>
         <v>0.1558441558441559</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M12" si="8">M4+J5</f>
+        <f t="shared" ref="M5:M11" si="8">M4+J5</f>
         <v>0.316</v>
       </c>
       <c r="N5">
@@ -1187,6 +3158,11 @@
         <v>0.46119480519480532</v>
       </c>
     </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>11</v>
@@ -1199,7 +3175,203 @@
         <v>0.53880519480519462</v>
       </c>
     </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>0.25974025974025972</v>
+      </c>
+      <c r="C23">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L23">
+        <v>0.1</v>
+      </c>
+      <c r="M23" s="11">
+        <v>0.25974025974025972</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="C24">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="L24">
+        <v>0.2</v>
+      </c>
+      <c r="M24" s="11">
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>0.70129870129870131</v>
+      </c>
+      <c r="C25">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.3</v>
+      </c>
+      <c r="M25" s="11">
+        <v>0.70129870129870131</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="C26">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="L26">
+        <v>0.4</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <v>0.8701298701298702</v>
+      </c>
+      <c r="C27">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="L27">
+        <v>0.5</v>
+      </c>
+      <c r="M27" s="11">
+        <v>0.8701298701298702</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <v>0.89610389610389618</v>
+      </c>
+      <c r="C28">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="L28">
+        <v>0.6</v>
+      </c>
+      <c r="M28" s="11">
+        <v>0.89610389610389618</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>0.92207792207792216</v>
+      </c>
+      <c r="C29">
+        <v>0.628</v>
+      </c>
+      <c r="L29">
+        <v>0.7</v>
+      </c>
+      <c r="M29" s="11">
+        <v>0.92207792207792216</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <v>0.97402597402597413</v>
+      </c>
+      <c r="C30">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="L30">
+        <v>0.8</v>
+      </c>
+      <c r="M30" s="11">
+        <v>0.97402597402597413</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="11">
+        <v>0.97402597402597413</v>
+      </c>
+      <c r="C31">
+        <v>0.876</v>
+      </c>
+      <c r="L31">
+        <v>0.9</v>
+      </c>
+      <c r="M31" s="11">
+        <v>0.97402597402597413</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" s="11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF636381-8676-44C7-A63B-5ED96D8012B6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>